<commit_message>
Trim intro and remove GWWA
</commit_message>
<xml_diff>
--- a/num pages.xlsx
+++ b/num pages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Current Length of DM manuscript</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>Observation process</t>
-  </si>
-  <si>
-    <t>Statistical Inference</t>
-  </si>
-  <si>
-    <t>Maximum likelihood</t>
   </si>
   <si>
     <t xml:space="preserve">Bayesian </t>
@@ -440,20 +434,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -461,15 +455,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <f>SUM(F4,F5,F6,F13,F20,F23,F26,F27,F28,F29,F30)</f>
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -477,115 +475,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:11">
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="F5">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="F6">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="F7">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="F8">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="F9">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12" t="s">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="F13">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="F14">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" t="s">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="F15">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0.5</v>
+      </c>
+      <c r="K15">
+        <f>141.5/56.2</f>
+        <v>2.5177935943060499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="F16">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="F17">
-        <v>0.5</v>
-      </c>
-      <c r="K17">
-        <f>141.5/56.2</f>
-        <v>2.5177935943060499</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="C18" t="s">
         <v>18</v>
       </c>
@@ -593,115 +591,99 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:6">
       <c r="C19" t="s">
         <v>19</v>
       </c>
       <c r="F19">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="C20" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
       <c r="C21" t="s">
         <v>21</v>
       </c>
       <c r="F21">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" t="s">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="F22">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="C23" t="s">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="F23">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
       <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="F24">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11">
-      <c r="B25" t="s">
+      <c r="F26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="F25">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11">
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
       <c r="F27">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="F28">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="F29">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
       <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="F30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Formatting and further trims
</commit_message>
<xml_diff>
--- a/num pages.xlsx
+++ b/num pages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Current Length of DM manuscript</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Figures</t>
+  </si>
+  <si>
+    <t>Words</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -454,6 +457,9 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
@@ -464,7 +470,10 @@
       </c>
       <c r="G3">
         <f>SUM(F4,F5,F6,F13,F20,F23,F26,F27,F28,F29,F30)</f>
-        <v>20.9</v>
+        <v>20.149999999999999</v>
+      </c>
+      <c r="H3">
+        <v>8370</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -544,7 +553,7 @@
         <v>13</v>
       </c>
       <c r="F13">
-        <v>3.2</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -652,7 +661,7 @@
         <v>24</v>
       </c>
       <c r="F26">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="27" spans="2:6">
@@ -668,7 +677,7 @@
         <v>26</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="29" spans="2:6">

</xml_diff>

<commit_message>
Incorporated comments from Richard plus formatted for Ecology
</commit_message>
<xml_diff>
--- a/num pages.xlsx
+++ b/num pages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Current Length of DM manuscript</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Observer effects</t>
   </si>
   <si>
-    <t>Forecasting</t>
-  </si>
-  <si>
     <t>Applications</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Earlier</t>
+  </si>
+  <si>
+    <t>Forecasting or Inference</t>
   </si>
 </sst>
 </file>
@@ -449,29 +449,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1">
         <v>41535</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1">
+        <v>41610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -479,16 +483,19 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -508,8 +515,11 @@
       <c r="J3" s="2">
         <v>8349</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -519,8 +529,11 @@
       <c r="I4">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -530,8 +543,11 @@
       <c r="I5">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -541,8 +557,11 @@
       <c r="I6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -552,8 +571,11 @@
       <c r="I7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -564,7 +586,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -574,8 +596,11 @@
       <c r="I9">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -585,8 +610,11 @@
       <c r="I10">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -596,8 +624,11 @@
       <c r="I11">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -608,7 +639,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -618,8 +649,11 @@
       <c r="I13">
         <v>2.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -629,8 +663,11 @@
       <c r="I14">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>15</v>
       </c>
@@ -644,8 +681,11 @@
         <f>141.5/56.2</f>
         <v>2.5177935943060499</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>16</v>
       </c>
@@ -655,8 +695,11 @@
       <c r="I16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>17</v>
       </c>
@@ -666,8 +709,11 @@
       <c r="I17">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>18</v>
       </c>
@@ -677,10 +723,13 @@
       <c r="I18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F19">
         <v>0.4</v>
@@ -688,10 +737,13 @@
       <c r="I19">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20">
         <v>1.1000000000000001</v>
@@ -699,10 +751,13 @@
       <c r="I20">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21">
         <v>0.4</v>
@@ -710,10 +765,13 @@
       <c r="I21">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22">
         <v>0.7</v>
@@ -721,10 +779,13 @@
       <c r="I22">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23">
         <v>0.95</v>
@@ -732,10 +793,13 @@
       <c r="I23">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <v>0.3</v>
@@ -743,10 +807,13 @@
       <c r="I24">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25">
         <v>0.6</v>
@@ -754,10 +821,13 @@
       <c r="I25">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F26">
         <v>2.1</v>
@@ -765,10 +835,13 @@
       <c r="I26">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F27">
         <v>0.1</v>
@@ -776,10 +849,13 @@
       <c r="I27">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28">
         <v>2.9</v>
@@ -787,10 +863,13 @@
       <c r="I28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -798,16 +877,28 @@
       <c r="I29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
       <c r="I30">
         <v>4</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f>L4+L5+L6+L13+L20+L23+L26+L27+L28+L29+L30</f>
+        <v>29.849999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Response to reviewer's comments
</commit_message>
<xml_diff>
--- a/num pages.xlsx
+++ b/num pages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Current Length of DM manuscript</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Forecasting or Inference</t>
+  </si>
+  <si>
+    <t>Robustness</t>
   </si>
 </sst>
 </file>
@@ -449,19 +452,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +477,11 @@
       <c r="L1" s="1">
         <v>41610</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1">
+        <v>41808</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -494,8 +500,11 @@
       <c r="L2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -503,7 +512,7 @@
         <v>21</v>
       </c>
       <c r="G3">
-        <f>SUM(F4,F5,F6,F13,F20,F23,F26,F27,F28,F29,F30)</f>
+        <f>SUM(F4,F5,F6,F13,F20,F24,F28,F29,F30,F31,F32)</f>
         <v>20.149999999999999</v>
       </c>
       <c r="H3">
@@ -518,8 +527,11 @@
       <c r="L3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -532,8 +544,11 @@
       <c r="L4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -546,8 +561,11 @@
       <c r="L5">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -560,8 +578,11 @@
       <c r="L6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -574,8 +595,11 @@
       <c r="L7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -586,7 +610,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -599,8 +623,11 @@
       <c r="L9">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>10</v>
       </c>
@@ -613,8 +640,11 @@
       <c r="L10">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -627,8 +657,11 @@
       <c r="L11">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -639,7 +672,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -652,8 +685,11 @@
       <c r="L13">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>14</v>
       </c>
@@ -666,8 +702,11 @@
       <c r="L14">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>15</v>
       </c>
@@ -684,8 +723,11 @@
       <c r="L15">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>16</v>
       </c>
@@ -698,8 +740,11 @@
       <c r="L16">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>17</v>
       </c>
@@ -712,8 +757,15 @@
       <c r="L17">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>1.5</v>
+      </c>
+      <c r="N17">
+        <f>SUM(M14:M19)</f>
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>18</v>
       </c>
@@ -726,8 +778,11 @@
       <c r="L18">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>30</v>
       </c>
@@ -740,8 +795,11 @@
       <c r="L19">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -754,8 +812,11 @@
       <c r="L20">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>20</v>
       </c>
@@ -768,137 +829,187 @@
       <c r="L21">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="F22">
-        <v>0.7</v>
-      </c>
-      <c r="I22">
-        <v>0.7</v>
-      </c>
-      <c r="L22">
+      <c r="F23">
+        <v>0.7</v>
+      </c>
+      <c r="I23">
+        <v>0.7</v>
+      </c>
+      <c r="L23">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="M23">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>0.95</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>0.95</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="M24">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>0.3</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>0.3</v>
       </c>
-      <c r="L24">
+      <c r="L25">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="M25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="M26">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <v>0.6</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <v>0.6</v>
       </c>
-      <c r="L25">
+      <c r="L27">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>23</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>2.1</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>2.1</v>
       </c>
-      <c r="L26">
+      <c r="L28">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="M28">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>24</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>0.1</v>
       </c>
-      <c r="I27">
+      <c r="I29">
         <v>0.1</v>
       </c>
-      <c r="L27">
+      <c r="L29">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="M29">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="F28">
+      <c r="F30">
         <v>2.9</v>
       </c>
-      <c r="I28">
+      <c r="I30">
         <v>3</v>
       </c>
-      <c r="L28">
+      <c r="L30">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="M30">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="F29">
+      <c r="F31">
         <v>1</v>
       </c>
-      <c r="I29">
+      <c r="I31">
         <v>1</v>
       </c>
-      <c r="L29">
+      <c r="L31">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>27</v>
       </c>
-      <c r="F30">
+      <c r="F32">
         <v>4</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <v>4</v>
       </c>
-      <c r="L30">
+      <c r="L32">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L32">
-        <f>L4+L5+L6+L13+L20+L23+L26+L27+L28+L29+L30</f>
+      <c r="M32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f>L4+L5+L6+L13+L20+L24+L28+L29+L30+L31+L32</f>
         <v>29.849999999999998</v>
+      </c>
+      <c r="M34">
+        <f>M4+M5+M6+M13+M20+M24+M28+M29+M30+M31+M32</f>
+        <v>30.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>